<commit_message>
Update genmap V2 021125
</commit_message>
<xml_diff>
--- a/data/curriculum_source.xlsx
+++ b/data/curriculum_source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Downloads/IOSTEM-JSONIMPORT-main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75ADD3A0-02D8-D943-B70D-2DF847E57FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6318AF35-690E-C54C-B53A-D6690CC4BF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="25100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="130">
   <si>
     <t>Grade</t>
   </si>
@@ -409,10 +409,7 @@
     <t>ALL Thu thập tất cả các loại kho báu khác nhau (pha lê, đá quý, chìa khóa) trong mê cung trước khi đến đích.</t>
   </si>
   <si>
-    <t>maze_width:14; items_to_place:['crystal','crystal', 'crystal']; asset_theme:{'ground':'stone.stone04'}</t>
-  </si>
-  <si>
-    <t>crystal:3</t>
+    <t>maze_width:12; items_to_place:['crystal','crystal']; asset_theme:{'ground':'wall.brick01'}</t>
   </si>
 </sst>
 </file>
@@ -711,8 +708,8 @@
   </sheetPr>
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1519,7 +1516,7 @@
         <v>28</v>
       </c>
       <c r="P15" s="8" t="s">
-        <v>130</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>